<commit_message>
feat: implement bid creation logic
</commit_message>
<xml_diff>
--- a/templates/bid.xlsx
+++ b/templates/bid.xlsx
@@ -1,48 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Stockwise\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352D094D-2FED-4B80-804A-C5982010AE82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFFEFF9-EC95-41E3-A6F5-3ED27DA97261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>Заявка о комплектовани</t>
-  </si>
-  <si>
-    <t>{{ whom_position }}</t>
-  </si>
-  <si>
-    <t>{{ whom_fio }}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Исх № {{ outgoing_number }} от {{ current_date }}</t>
-  </si>
-  <si>
-    <t>Приложение: перечень</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          Обеспечить наличие на складе комплектации согласно приложенного перечня под план проихводства на {{ current_month }} в срок до _______________________</t>
   </si>
   <si>
     <t>{{ from_position }}</t>
@@ -51,14 +31,20 @@
     <t>{{ from_fio }}</t>
   </si>
   <si>
-    <t>подпись</t>
+    <t>Заявка о комплектовании</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        Обеспечить наличие на складе комплектации материалов для изготовления изделия {{ product_name }} в количестве, рассчитанном на {{ product_quantity }} шт., согласно приложенному перечню, под план производства на _______________ в срок до ____________________</t>
+  </si>
+  <si>
+    <t>{{ whom_position }}{{ '\n' }}{{ whom_fio }}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -73,13 +59,6 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -89,7 +68,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -97,44 +76,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -415,110 +382,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="8" style="1" customWidth="1"/>
+    <col min="2" max="9" width="10" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="G1" s="3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="G20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="9"/>
-      <c r="I14" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E15" s="8" t="s">
-        <v>8</v>
-      </c>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A6:I8"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="G2:I2"/>
+  <mergeCells count="6">
+    <mergeCell ref="G20:I22"/>
+    <mergeCell ref="A20:E22"/>
+    <mergeCell ref="A9:I14"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E1:I5"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1"/>
+  <pageMargins left="0.78740157480314965" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" fitToWidth="0" fitToHeight="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(excel): generate workbook with document sheet and materials list sheet
</commit_message>
<xml_diff>
--- a/templates/bid.xlsx
+++ b/templates/bid.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Python Projects\Stockwise\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Projects\Stockwise\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFFEFF9-EC95-41E3-A6F5-3ED27DA97261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2872BB5-FDAF-450F-B32A-F9092F9835B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -80,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -102,6 +102,9 @@
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -385,72 +388,72 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="F1" sqref="F1:I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8" defaultRowHeight="18" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="8" style="1" customWidth="1"/>
     <col min="2" max="9" width="10" style="1" customWidth="1"/>
     <col min="10" max="16384" width="8" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="8"/>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E3" s="3"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E4" s="3"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="E5" s="3"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A9" s="7" t="s">
         <v>4</v>
       </c>
@@ -463,7 +466,7 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -474,7 +477,7 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -485,7 +488,7 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -496,7 +499,7 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -507,7 +510,7 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
     </row>
-    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -518,7 +521,7 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -529,11 +532,11 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="6" t="s">
         <v>1</v>
       </c>
@@ -547,7 +550,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="6"/>
       <c r="B21" s="6"/>
       <c r="C21" s="6"/>
@@ -557,7 +560,7 @@
       <c r="H21" s="5"/>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="6"/>
       <c r="B22" s="6"/>
       <c r="C22" s="6"/>
@@ -574,7 +577,7 @@
     <mergeCell ref="A9:I14"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E1:I5"/>
+    <mergeCell ref="F1:I5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.78740157480314965" right="0.19685039370078741" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>